<commit_message>
python stdev.p -> stdev.s
</commit_message>
<xml_diff>
--- a/results/python/awesome-python/awesome-python.xlsx
+++ b/results/python/awesome-python/awesome-python.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamc\Desktop\results\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashort11/research/CodeSize/results/python/awesome-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1D4977E-E07B-4515-85B5-F3703BFF92C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3BF040-D6B6-7044-BDCD-9EE5E7FB33FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="12105"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="23980" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="awesome-python" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -79,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -915,16 +923,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -994,15 +1002,15 @@
         <v>30</v>
       </c>
       <c r="N2" s="2">
-        <f>_xlfn.STDEV.P(C2:C3)</f>
-        <v>3</v>
+        <f>_xlfn.STDEV.S(C2:C3)</f>
+        <v>4.2426406871192848</v>
       </c>
       <c r="O2" s="2">
         <f>N2/SQRT(COUNT(C2:C3))</f>
-        <v>2.1213203435596424</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1037,15 +1045,15 @@
         <v>29</v>
       </c>
       <c r="N3" s="2">
-        <f>_xlfn.STDEV.P(D2:D3)</f>
-        <v>11</v>
+        <f>_xlfn.STDEV.S(D2:D3)</f>
+        <v>15.556349186104045</v>
       </c>
       <c r="O3" s="2">
         <f>N3/SQRT(COUNT(D2:D3))</f>
-        <v>7.7781745930520225</v>
+        <v>10.999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="N4" s="2">
-        <f>_xlfn.STDEV.P(E2:E3)</f>
+        <f>_xlfn.STDEV.S(E2:E3)</f>
         <v>0</v>
       </c>
       <c r="O4" s="2">
@@ -1070,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1087,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <f>_xlfn.STDEV.P(F2:F3)</f>
+        <f>_xlfn.STDEV.S(F2:F3)</f>
         <v>0</v>
       </c>
       <c r="O5" s="2">

</xml_diff>